<commit_message>
0.2.22 Example Videos TOI-4504
</commit_message>
<xml_diff>
--- a/research/star_systems/TOI-4504.xlsx
+++ b/research/star_systems/TOI-4504.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive.aspit.dk/personal/ulsc/Documents/Uli/Python/curvesim/research/star_systems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{D9065C37-32B8-40B0-941F-9D48DBE89851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA0A7500-349A-46AB-9964-CE60E297BED9}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="13_ncr:1_{D9065C37-32B8-40B0-941F-9D48DBE89851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD53358-EDA3-417E-AE70-27CC047E3DCC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{6919DDE8-15F9-45FB-B5F7-4209377AF865}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>[TOI-4504]</t>
   </si>
@@ -188,15 +188,9 @@
     <t>ppm</t>
   </si>
   <si>
-    <t>Uli ppm</t>
-  </si>
-  <si>
     <t>pi * r^2</t>
   </si>
   <si>
-    <t>/ statt * mean_intensity in total_luminosity()</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">def </t>
     </r>
@@ -1578,9 +1572,6 @@
     <t xml:space="preserve">    float: intensity relative to the intensity at the midlle of the star at the given relative radius.</t>
   </si>
   <si>
-    <t xml:space="preserve">    """</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">    </t>
     </r>
@@ -2049,28 +2040,40 @@
     <t>TOI-4504</t>
   </si>
   <si>
-    <t>[0.4765, 0.3495]</t>
-  </si>
-  <si>
     <t>limb_darkening</t>
   </si>
   <si>
     <t>luminosity</t>
   </si>
   <si>
-    <t>0.7095</t>
-  </si>
-  <si>
     <t>mean_intensity</t>
   </si>
   <si>
     <t>area_2d</t>
   </si>
   <si>
-    <t>luminosity per area</t>
-  </si>
-  <si>
     <t>mean intensity /central intensity  (based on the given coefficients</t>
+  </si>
+  <si>
+    <t>[0.4765, 0.3495, 0.174]</t>
+  </si>
+  <si>
+    <t>mean brightness  (luminosity per area)</t>
+  </si>
+  <si>
+    <t>brightness at center</t>
+  </si>
+  <si>
+    <t>Uli [0.4765, 0.3495]</t>
+  </si>
+  <si>
+    <t>Uli [0.4765, 0.3495, 0.174]</t>
+  </si>
+  <si>
+    <t>total luminosity</t>
+  </si>
+  <si>
+    <t>total area</t>
   </si>
 </sst>
 </file>
@@ -2078,7 +2081,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2226,7 +2229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2264,7 +2267,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2274,6 +2277,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3109,10 +3113,14 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
@@ -3120,16 +3128,16 @@
         <v>14</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
         <v>16</v>
       </c>
       <c r="N1" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="O1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -3230,14 +3238,14 @@
         <v>717.78433235625619</v>
       </c>
       <c r="N11" s="5">
-        <v>409</v>
+        <v>859</v>
       </c>
       <c r="O11">
         <v>812</v>
       </c>
       <c r="P11">
         <f>N11/M11</f>
-        <v>0.56980903812344852</v>
+        <v>1.196738297672475</v>
       </c>
       <c r="Q11">
         <f>O11/M11</f>
@@ -3265,35 +3273,46 @@
         <v>12198.353034358604</v>
       </c>
       <c r="N13">
-        <v>6845</v>
+        <v>14270.000000000067</v>
       </c>
       <c r="O13">
         <v>13598</v>
       </c>
       <c r="P13">
         <f>N13/M13</f>
-        <v>0.56114132626920754</v>
+        <v>1.1698300549103915</v>
       </c>
       <c r="Q13">
         <f>O13/M13</f>
         <v>1.1147406507828612</v>
       </c>
     </row>
-    <row r="19" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M19">
-        <v>99.918800000000005</v>
-      </c>
-    </row>
-    <row r="20" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M20">
-        <f>100-M19</f>
-        <v>8.1199999999995498E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M21">
-        <f>M20*10000</f>
-        <v>811.99999999995498</v>
+    <row r="19" spans="14:15" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>98.572999999999993</v>
+      </c>
+      <c r="O19">
+        <v>99.914100000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="14:15" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <f>100-N19</f>
+        <v>1.4270000000000067</v>
+      </c>
+      <c r="O20">
+        <f>100-O19</f>
+        <v>8.5899999999995202E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="14:15" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <f>N20*10000</f>
+        <v>14270.000000000067</v>
+      </c>
+      <c r="O21">
+        <f>O20*10000</f>
+        <v>858.99999999995202</v>
       </c>
     </row>
   </sheetData>
@@ -3303,22 +3322,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E359EDAB-6C8B-452C-B771-172741AC8B82}">
-  <dimension ref="A1:AC49"/>
+  <dimension ref="A1:AC50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3351,7 +3370,7 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3384,7 +3403,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -3417,7 +3436,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -3450,7 +3469,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3483,7 +3502,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3516,7 +3535,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -3549,7 +3568,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -3582,7 +3601,7 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -3615,7 +3634,7 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -3648,7 +3667,7 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -3681,7 +3700,7 @@
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -3714,7 +3733,7 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -3747,7 +3766,7 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -3780,7 +3799,7 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -3813,7 +3832,7 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -3846,7 +3865,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -3878,8 +3897,8 @@
       <c r="AC20" s="7"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>51</v>
+      <c r="A21" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -3911,8 +3930,8 @@
       <c r="AC21" s="7"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A22" s="12" t="s">
-        <v>52</v>
+      <c r="A22" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -3944,8 +3963,8 @@
       <c r="AC22" s="7"/>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>53</v>
+      <c r="A23" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -3977,8 +3996,8 @@
       <c r="AC23" s="7"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>54</v>
+      <c r="A24" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -4010,8 +4029,8 @@
       <c r="AC24" s="7"/>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>55</v>
+      <c r="A25" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -4043,8 +4062,8 @@
       <c r="AC25" s="7"/>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
-        <v>56</v>
+      <c r="A26" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -4075,42 +4094,42 @@
       <c r="AB26" s="7"/>
       <c r="AC26" s="7"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A27" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-      <c r="V27" s="7"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="7"/>
-      <c r="AC27" s="7"/>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
+      <c r="AB28" s="7"/>
+      <c r="AC28" s="7"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>20</v>
+      <c r="A29" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -4142,8 +4161,8 @@
       <c r="AC29" s="7"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>21</v>
+      <c r="A30" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -4176,7 +4195,7 @@
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -4208,8 +4227,8 @@
       <c r="AC31" s="7"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>23</v>
+      <c r="A32" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -4241,8 +4260,8 @@
       <c r="AC32" s="7"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>24</v>
+      <c r="A33" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -4274,8 +4293,8 @@
       <c r="AC33" s="7"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>25</v>
+      <c r="A34" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -4307,8 +4326,8 @@
       <c r="AC34" s="7"/>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
-        <v>26</v>
+      <c r="A35" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -4340,8 +4359,8 @@
       <c r="AC35" s="7"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
-        <v>27</v>
+      <c r="A36" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -4373,8 +4392,8 @@
       <c r="AC36" s="7"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
-        <v>28</v>
+      <c r="A37" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -4406,8 +4425,8 @@
       <c r="AC37" s="7"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
-        <v>29</v>
+      <c r="A38" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -4439,8 +4458,8 @@
       <c r="AC38" s="7"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
-        <v>30</v>
+      <c r="A39" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -4473,7 +4492,7 @@
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -4506,7 +4525,7 @@
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -4537,95 +4556,88 @@
       <c r="AB41" s="7"/>
       <c r="AC41" s="7"/>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A42" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="7"/>
-      <c r="V42" s="7"/>
-      <c r="W42" s="7"/>
-      <c r="X42" s="7"/>
-      <c r="Y42" s="7"/>
-      <c r="Z42" s="7"/>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="7"/>
-      <c r="AC42" s="7"/>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
-        <v>58</v>
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="17">
+        <v>2.3745999999999999E+26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" s="17">
-        <v>2.3745999999999999E+26</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1.28934965510609E+18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1.28934965510609E+18</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="F46" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="B46" s="15">
+        <f>B44/B45</f>
+        <v>184170367.64201978</v>
+      </c>
+      <c r="C46" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="15">
-        <f>B45/B46</f>
-        <v>184170367.64201978</v>
-      </c>
-      <c r="C47" t="s">
-        <v>65</v>
+        <v>56</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47">
+        <v>0.47649999999999998</v>
+      </c>
+      <c r="H47">
+        <v>0.34949999999999998</v>
+      </c>
+      <c r="I47">
+        <f>1-G47-H47</f>
+        <v>0.1740000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="16">
+        <v>0.79649999999999999</v>
+      </c>
+      <c r="C48" t="s">
         <v>60</v>
       </c>
-      <c r="B48" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" t="s">
-        <v>66</v>
+      <c r="B50" s="19">
+        <f>B46/B48</f>
+        <v>231224567.03329539</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
0.3.0 limb darkening alternative models
</commit_message>
<xml_diff>
--- a/research/star_systems/TOI-4504.xlsx
+++ b/research/star_systems/TOI-4504.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Python\curvesim\research\star_systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80347970-C0E4-46C4-AAC8-FB743D815952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C37966-8715-4B88-B8EB-7DB88EDDCBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6919DDE8-15F9-45FB-B5F7-4209377AF865}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>[TOI-4504]</t>
   </si>
@@ -2074,14 +2074,50 @@
   </si>
   <si>
     <t>area ppm</t>
+  </si>
+  <si>
+    <t>P [days]</t>
+  </si>
+  <si>
+    <t>T0 [BJD]</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>start_date - T0</t>
+  </si>
+  <si>
+    <t>(start_date - T0) / P</t>
+  </si>
+  <si>
+    <t>T0 - 263* P</t>
+  </si>
+  <si>
+    <t>first transit in simulation</t>
+  </si>
+  <si>
+    <t>Given q1 and q2 and the relative_radius r (the normalized radial coordinate (0 &lt;= r &lt;= 1), what is the formula for the limb darkening?</t>
+  </si>
+  <si>
+    <t>What do the parameters q1 and q2 (no units given) describe in the context of exoplanets?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+the english wikipedia article on limb darkening uses parameters a0, a1, a2 or alternatively A1 and A2. What is the relationship between these paramers and the parameters you mentioned (u1, u2 and q1, q2)?</t>
+  </si>
+  <si>
+    <t>You called u1, u2 the quadratic law parameters. Give me names for the 3 other parameter sets q1, q2 and a0, a1, a2 and A1, A2.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="172" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="175" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2229,7 +2265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2278,6 +2314,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2301,6 +2343,187 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400967</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>96017</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B25C84F-A280-0EE6-8781-0723DD4D7F58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="552450" y="7553325"/>
+          <a:ext cx="6573167" cy="5496692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>286654</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>47723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9CC761A-B11B-4F19-1600-0CFD140B4173}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="533400" y="6391275"/>
+          <a:ext cx="6477904" cy="704948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>48532</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>10468</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A981E6EA-CE0F-19D3-B8FF-B852399628F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="13449300"/>
+          <a:ext cx="6496957" cy="6754168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>572355</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>38424</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1AE8F4B-BBC9-CD62-1020-B90DCE65462D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="400050" y="20764500"/>
+          <a:ext cx="6125430" cy="2324424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3226,14 +3449,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C734D42E-A664-47EC-9C8A-1146EAD8C69E}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="K112" sqref="K112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3387,7 +3612,7 @@
         <v>13598</v>
       </c>
     </row>
-    <row r="19" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N19">
         <v>98.572999999999993</v>
       </c>
@@ -3395,7 +3620,7 @@
         <v>99.914100000000005</v>
       </c>
     </row>
-    <row r="20" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N20">
         <f>100-N19</f>
         <v>1.4270000000000067</v>
@@ -3405,7 +3630,7 @@
         <v>8.5899999999995202E-2</v>
       </c>
     </row>
-    <row r="21" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N21">
         <f>N20*10000</f>
         <v>14270.000000000067</v>
@@ -3415,8 +3640,104 @@
         <v>858.99999999995202</v>
       </c>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="20">
+        <v>2.4261400000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="21">
+        <v>2459038.4580000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="21">
+        <v>2458400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="21">
+        <f>B26-B27</f>
+        <v>638.45800000010058</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="21">
+        <f>B28/B25</f>
+        <v>263.15793812397493</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="21">
+        <f>B26-B25*ROUNDDOWN(B29,0)</f>
+        <v>2458400.3831799999</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
0.3.3 Improved orbit simulation using Verlet integration
</commit_message>
<xml_diff>
--- a/research/star_systems/TOI-4504.xlsx
+++ b/research/star_systems/TOI-4504.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Python\curvesim\research\star_systems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE158D5C-B750-4A2A-B862-D517B9BBA874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D481EAF8-63E0-4921-BDDC-BA7B803C24AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6919DDE8-15F9-45FB-B5F7-4209377AF865}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
   <si>
     <t>[TOI-4504]</t>
   </si>
@@ -2174,18 +2174,37 @@
       <t>. Sollwert 0,3830000. Mit und ohne genauer berechnetem Minimum zwischen Iterationsschritten.</t>
     </r>
   </si>
+  <si>
+    <t>Ø</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>max Fehler +</t>
+  </si>
+  <si>
+    <t>max Fehler -</t>
+  </si>
+  <si>
+    <t>TT von Planet c</t>
+  </si>
+  <si>
+    <t>Loesung: Verlet Integration!!!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0000%"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="179" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2311,6 +2330,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2339,7 +2366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2397,7 +2424,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -2839,7 +2872,899 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>P von Planet b: Abweichungen vom Mittelwert waehrend der Simulation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.6361694507032516E-2"/>
+                  <c:y val="-0.1856374346336479"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="de-DE"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>'TOI 4504'!$C$149:$C$207</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="59"/>
+                <c:pt idx="0">
+                  <c:v>3.2656334298941658E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2894508973984102E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0835446397905457E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0048631098900103E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4384090000247909E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.514792679685911E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.8158503097623964E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.1716155399268473E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.5341252300530357E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.0016339397405147E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0034813496857566E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.4914791497975273E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6973014396757264E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.9771791098839344E-6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.5532173499380804E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.6836025099401581E-6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0116380398156366E-6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.0416503498109648E-6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9943781097708779E-6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0472382896995498E-6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.1748447096322536E-6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.3252685299785014E-6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.8610194599603176E-6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.4840742597135375E-6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.0752236499014316E-6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.6302766798264088E-6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.3760103799760373E-6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.0351310900122996E-6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.9394300796449215E-6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2619081400397931E-6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.2104754099401305E-6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.7033854997132778E-6</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.9797708990293472E-7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.7993042978357039E-7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.5845961800486918E-6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.7010267299741884E-6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.1862610198915036E-6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8.556011309668321E-6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0270110510024466E-5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.0721801960045241E-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9.4598598696649105E-6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.7911550396537734E-6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.3166309500186628E-6</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.1615657497828806E-6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.500582389712406E-6</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.5914015697241553E-6</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.9203836600427735E-6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.1101177898082994E-6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.4521231596352777E-6</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.3494372299582835E-6</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.8830850696538448E-6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.539442269939741E-6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.7545930096658537E-6</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>8.0475091897014295E-6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>9.9478728996515997E-6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.0881523779815439E-5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.0217490789887762E-5</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>7.7047824800224873E-6</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.2970731799485407E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C6EB-4AD5-AF2A-3B12205E2CBB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="676869440"/>
+        <c:axId val="676860320"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="676869440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="676860320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="676860320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="676869440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>P von Planet c</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'TOI 4504'!$B$218:$B$228</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>82.622222220059484</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.712499999906868</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.931944449897856</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.193055550102144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83.404166670050472</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83.50833333004266</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.511111109983176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.434722229838371</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83.298611110076308</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>83.126388890203089</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>82.940277769695967</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A54-4EFF-B983-41B25F81D9A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="871048880"/>
+        <c:axId val="871047440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="871048880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="871047440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="871047440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="871048880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3395,6 +4320,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -3405,8 +5362,8 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>115217</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>315242</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>96017</xdr:rowOff>
     </xdr:to>
@@ -3449,8 +5406,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>904</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>200929</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>47723</xdr:rowOff>
     </xdr:to>
@@ -3493,8 +5450,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>534307</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>734332</xdr:colOff>
       <xdr:row>106</xdr:row>
       <xdr:rowOff>10468</xdr:rowOff>
     </xdr:to>
@@ -3537,8 +5494,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>286605</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>486630</xdr:colOff>
       <xdr:row>121</xdr:row>
       <xdr:rowOff>38424</xdr:rowOff>
     </xdr:to>
@@ -3604,6 +5561,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Diagramm 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A27C9D8-2545-38F3-AA87-BF6C8DD56616}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>890587</xdr:colOff>
+      <xdr:row>214</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>229</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Diagramm 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA3600CC-11F3-B098-8788-4CD35686CCF9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4538,16 +6567,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C734D42E-A664-47EC-9C8A-1146EAD8C69E}">
-  <dimension ref="A1:O145"/>
+  <dimension ref="A1:O228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="N146" sqref="N146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" customWidth="1"/>
     <col min="4" max="6" width="12.140625" customWidth="1"/>
     <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -4841,12 +6870,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="22" t="s">
         <v>84</v>
       </c>
@@ -4860,7 +6889,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="22">
         <v>120</v>
       </c>
@@ -4871,14 +6900,14 @@
         <v>0.38272699999999998</v>
       </c>
       <c r="D132" s="23">
-        <f>($F$132-C132)/$F$132</f>
+        <f t="shared" ref="D132:D138" si="0">($F$132-C132)/$F$132</f>
         <v>7.1279373368152274E-4</v>
       </c>
       <c r="F132">
         <v>0.38300000000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="22">
         <v>60</v>
       </c>
@@ -4889,11 +6918,11 @@
         <v>0.38284400000000002</v>
       </c>
       <c r="D133" s="23">
-        <f>($F$132-C133)/$F$132</f>
+        <f t="shared" si="0"/>
         <v>4.0731070496080802E-4</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="22">
         <v>20</v>
       </c>
@@ -4904,11 +6933,11 @@
         <v>0.38292199999999998</v>
       </c>
       <c r="D134" s="23">
-        <f>($F$132-C134)/$F$132</f>
+        <f t="shared" si="0"/>
         <v>2.0365535248047649E-4</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="22">
         <v>10</v>
       </c>
@@ -4919,11 +6948,11 @@
         <v>0.38294099999999998</v>
       </c>
       <c r="D135" s="23">
-        <f>($F$132-C135)/$F$132</f>
+        <f t="shared" si="0"/>
         <v>1.5404699738911552E-4</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="16">
         <v>5</v>
       </c>
@@ -4934,11 +6963,11 @@
         <v>0.38295099999999999</v>
       </c>
       <c r="D136" s="23">
-        <f>($F$132-C136)/$F$132</f>
+        <f t="shared" si="0"/>
         <v>1.2793733681467688E-4</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="16">
         <v>1</v>
       </c>
@@ -4949,11 +6978,11 @@
         <v>0.38295899999999999</v>
       </c>
       <c r="D137" s="23">
-        <f>($F$132-C137)/$F$132</f>
+        <f t="shared" si="0"/>
         <v>1.0704960835512597E-4</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="22">
         <v>0.1</v>
       </c>
@@ -4964,11 +6993,11 @@
         <v>0.382961</v>
       </c>
       <c r="D138" s="23">
-        <f>($F$132-C138)/$F$132</f>
+        <f t="shared" si="0"/>
         <v>1.0182767624023824E-4</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="18" t="s">
         <v>85</v>
       </c>
@@ -4976,29 +7005,919 @@
         <v>86</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B144" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H144" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C147">
+        <v>0.38275274869999998</v>
+      </c>
+      <c r="E147">
+        <f>F132-C147</f>
+        <v>2.4725130000002871E-4</v>
+      </c>
+      <c r="F147" s="23">
+        <f>E147/F132</f>
+        <v>6.455647519582995E-4</v>
+      </c>
+      <c r="I147">
+        <v>2.4261400000000002</v>
+      </c>
+      <c r="J147" s="23">
+        <f>1-I147/A149</f>
+        <v>1.46467459193107E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>2.4622032656334301</v>
+      </c>
+      <c r="B149">
+        <f>A149-2.4622</f>
+        <v>3.2656334298941658E-6</v>
+      </c>
+      <c r="C149">
+        <v>3.2656334298941658E-6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>2.4622009289450899</v>
+      </c>
+      <c r="B150">
+        <f t="shared" ref="B150:B207" si="1">A150-2.4622</f>
+        <v>9.2894508973984102E-7</v>
+      </c>
+      <c r="C150">
+        <v>9.2894508973984102E-7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>2.46220108354464</v>
+      </c>
+      <c r="B151">
+        <f t="shared" si="1"/>
+        <v>1.0835446397905457E-6</v>
+      </c>
+      <c r="C151">
+        <v>1.0835446397905457E-6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>2.4622030048631101</v>
+      </c>
+      <c r="B152">
+        <f t="shared" si="1"/>
+        <v>3.0048631098900103E-6</v>
+      </c>
+      <c r="C152">
+        <v>3.0048631098900103E-6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>2.4622054384090002</v>
+      </c>
+      <c r="B153">
+        <f t="shared" si="1"/>
+        <v>5.4384090000247909E-6</v>
+      </c>
+      <c r="C153">
+        <v>5.4384090000247909E-6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>2.4622075147926799</v>
+      </c>
+      <c r="B154">
+        <f t="shared" si="1"/>
+        <v>7.514792679685911E-6</v>
+      </c>
+      <c r="C154">
+        <v>7.514792679685911E-6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>2.4622088158503099</v>
+      </c>
+      <c r="B155">
+        <f t="shared" si="1"/>
+        <v>8.8158503097623964E-6</v>
+      </c>
+      <c r="C155">
+        <v>8.8158503097623964E-6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>2.4622091716155401</v>
+      </c>
+      <c r="B156">
+        <f t="shared" si="1"/>
+        <v>9.1716155399268473E-6</v>
+      </c>
+      <c r="C156">
+        <v>9.1716155399268473E-6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>2.4622085341252302</v>
+      </c>
+      <c r="B157">
+        <f t="shared" si="1"/>
+        <v>8.5341252300530357E-6</v>
+      </c>
+      <c r="C157">
+        <v>8.5341252300530357E-6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>2.4622070016339399</v>
+      </c>
+      <c r="B158">
+        <f t="shared" si="1"/>
+        <v>7.0016339397405147E-6</v>
+      </c>
+      <c r="C158">
+        <v>7.0016339397405147E-6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>2.4622050034813499</v>
+      </c>
+      <c r="B159">
+        <f t="shared" si="1"/>
+        <v>5.0034813496857566E-6</v>
+      </c>
+      <c r="C159">
+        <v>5.0034813496857566E-6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>2.46220349147915</v>
+      </c>
+      <c r="B160">
+        <f t="shared" si="1"/>
+        <v>3.4914791497975273E-6</v>
+      </c>
+      <c r="C160">
+        <v>3.4914791497975273E-6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>2.4622036973014398</v>
+      </c>
+      <c r="B161">
+        <f t="shared" si="1"/>
+        <v>3.6973014396757264E-6</v>
+      </c>
+      <c r="C161">
+        <v>3.6973014396757264E-6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>2.4622059771791101</v>
+      </c>
+      <c r="B162">
+        <f t="shared" si="1"/>
+        <v>5.9771791098839344E-6</v>
+      </c>
+      <c r="C162">
+        <v>5.9771791098839344E-6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>2.4622085532173501</v>
+      </c>
+      <c r="B163">
+        <f t="shared" si="1"/>
+        <v>8.5532173499380804E-6</v>
+      </c>
+      <c r="C163">
+        <v>8.5532173499380804E-6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>2.4622086836025101</v>
+      </c>
+      <c r="B164">
+        <f t="shared" si="1"/>
+        <v>8.6836025099401581E-6</v>
+      </c>
+      <c r="C164">
+        <v>8.6836025099401581E-6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>2.46220601163804</v>
+      </c>
+      <c r="B165">
+        <f t="shared" si="1"/>
+        <v>6.0116380398156366E-6</v>
+      </c>
+      <c r="C165">
+        <v>6.0116380398156366E-6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>2.46220304165035</v>
+      </c>
+      <c r="B166">
+        <f t="shared" si="1"/>
+        <v>3.0416503498109648E-6</v>
+      </c>
+      <c r="C166">
+        <v>3.0416503498109648E-6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>2.4622019943781099</v>
+      </c>
+      <c r="B167">
+        <f t="shared" si="1"/>
+        <v>1.9943781097708779E-6</v>
+      </c>
+      <c r="C167">
+        <v>1.9943781097708779E-6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>2.4622030472382899</v>
+      </c>
+      <c r="B168">
+        <f t="shared" si="1"/>
+        <v>3.0472382896995498E-6</v>
+      </c>
+      <c r="C168">
+        <v>3.0472382896995498E-6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>2.4622051748447098</v>
+      </c>
+      <c r="B169">
+        <f t="shared" si="1"/>
+        <v>5.1748447096322536E-6</v>
+      </c>
+      <c r="C169">
+        <v>5.1748447096322536E-6</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>2.4622073252685301</v>
+      </c>
+      <c r="B170">
+        <f t="shared" si="1"/>
+        <v>7.3252685299785014E-6</v>
+      </c>
+      <c r="C170">
+        <v>7.3252685299785014E-6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>2.4622088610194601</v>
+      </c>
+      <c r="B171">
+        <f t="shared" si="1"/>
+        <v>8.8610194599603176E-6</v>
+      </c>
+      <c r="C171">
+        <v>8.8610194599603176E-6</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>2.4622094840742599</v>
+      </c>
+      <c r="B172">
+        <f t="shared" si="1"/>
+        <v>9.4840742597135375E-6</v>
+      </c>
+      <c r="C172">
+        <v>9.4840742597135375E-6</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>2.4622090752236501</v>
+      </c>
+      <c r="B173">
+        <f t="shared" si="1"/>
+        <v>9.0752236499014316E-6</v>
+      </c>
+      <c r="C173">
+        <v>9.0752236499014316E-6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>2.46220763027668</v>
+      </c>
+      <c r="B174">
+        <f t="shared" si="1"/>
+        <v>7.6302766798264088E-6</v>
+      </c>
+      <c r="C174">
+        <v>7.6302766798264088E-6</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>2.4622053760103801</v>
+      </c>
+      <c r="B175">
+        <f t="shared" si="1"/>
+        <v>5.3760103799760373E-6</v>
+      </c>
+      <c r="C175">
+        <v>5.3760103799760373E-6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>2.4622030351310902</v>
+      </c>
+      <c r="B176">
+        <f t="shared" si="1"/>
+        <v>3.0351310900122996E-6</v>
+      </c>
+      <c r="C176">
+        <v>3.0351310900122996E-6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>2.4622019394300798</v>
+      </c>
+      <c r="B177">
+        <f t="shared" si="1"/>
+        <v>1.9394300796449215E-6</v>
+      </c>
+      <c r="C177">
+        <v>1.9394300796449215E-6</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>2.4622032619081402</v>
+      </c>
+      <c r="B178">
+        <f t="shared" si="1"/>
+        <v>3.2619081400397931E-6</v>
+      </c>
+      <c r="C178">
+        <v>3.2619081400397931E-6</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>2.4622062104754101</v>
+      </c>
+      <c r="B179">
+        <f t="shared" si="1"/>
+        <v>6.2104754099401305E-6</v>
+      </c>
+      <c r="C179">
+        <v>6.2104754099401305E-6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>2.4622077033854999</v>
+      </c>
+      <c r="B180">
+        <f t="shared" si="1"/>
+        <v>7.7033854997132778E-6</v>
+      </c>
+      <c r="C180">
+        <v>7.7033854997132778E-6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>2.4622006979770901</v>
+      </c>
+      <c r="B181">
+        <f t="shared" si="1"/>
+        <v>6.9797708990293472E-7</v>
+      </c>
+      <c r="C181">
+        <v>6.9797708990293472E-7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>2.4622003799304299</v>
+      </c>
+      <c r="B182">
+        <f t="shared" si="1"/>
+        <v>3.7993042978357039E-7</v>
+      </c>
+      <c r="C182">
+        <v>3.7993042978357039E-7</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>2.4622015845961802</v>
+      </c>
+      <c r="B183">
+        <f t="shared" si="1"/>
+        <v>1.5845961800486918E-6</v>
+      </c>
+      <c r="C183">
+        <v>1.5845961800486918E-6</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>2.4622037010267301</v>
+      </c>
+      <c r="B184">
+        <f t="shared" si="1"/>
+        <v>3.7010267299741884E-6</v>
+      </c>
+      <c r="C184">
+        <v>3.7010267299741884E-6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>2.4622061862610201</v>
+      </c>
+      <c r="B185">
+        <f t="shared" si="1"/>
+        <v>6.1862610198915036E-6</v>
+      </c>
+      <c r="C185">
+        <v>6.1862610198915036E-6</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>2.4622085560113098</v>
+      </c>
+      <c r="B186">
+        <f t="shared" si="1"/>
+        <v>8.556011309668321E-6</v>
+      </c>
+      <c r="C186">
+        <v>8.556011309668321E-6</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>2.4622102701105102</v>
+      </c>
+      <c r="B187">
+        <f t="shared" si="1"/>
+        <v>1.0270110510024466E-5</v>
+      </c>
+      <c r="C187">
+        <v>1.0270110510024466E-5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>2.4622107218019602</v>
+      </c>
+      <c r="B188">
+        <f t="shared" si="1"/>
+        <v>1.0721801960045241E-5</v>
+      </c>
+      <c r="C188">
+        <v>1.0721801960045241E-5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>2.4622094598598698</v>
+      </c>
+      <c r="B189">
+        <f t="shared" si="1"/>
+        <v>9.4598598696649105E-6</v>
+      </c>
+      <c r="C189">
+        <v>9.4598598696649105E-6</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>2.4622067911550398</v>
+      </c>
+      <c r="B190">
+        <f t="shared" si="1"/>
+        <v>6.7911550396537734E-6</v>
+      </c>
+      <c r="C190">
+        <v>6.7911550396537734E-6</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>2.4622043166309502</v>
+      </c>
+      <c r="B191">
+        <f t="shared" si="1"/>
+        <v>4.3166309500186628E-6</v>
+      </c>
+      <c r="C191">
+        <v>4.3166309500186628E-6</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>2.4622041615657499</v>
+      </c>
+      <c r="B192">
+        <f t="shared" si="1"/>
+        <v>4.1615657497828806E-6</v>
+      </c>
+      <c r="C192">
+        <v>4.1615657497828806E-6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>2.4622065005823899</v>
+      </c>
+      <c r="B193">
+        <f t="shared" si="1"/>
+        <v>6.500582389712406E-6</v>
+      </c>
+      <c r="C193">
+        <v>6.500582389712406E-6</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>2.4622085914015699</v>
+      </c>
+      <c r="B194">
+        <f t="shared" si="1"/>
+        <v>8.5914015697241553E-6</v>
+      </c>
+      <c r="C194">
+        <v>8.5914015697241553E-6</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>2.4622079203836602</v>
+      </c>
+      <c r="B195">
+        <f t="shared" si="1"/>
+        <v>7.9203836600427735E-6</v>
+      </c>
+      <c r="C195">
+        <v>7.9203836600427735E-6</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>2.46220511011779</v>
+      </c>
+      <c r="B196">
+        <f t="shared" si="1"/>
+        <v>5.1101177898082994E-6</v>
+      </c>
+      <c r="C196">
+        <v>5.1101177898082994E-6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>2.4622024521231598</v>
+      </c>
+      <c r="B197">
+        <f t="shared" si="1"/>
+        <v>2.4521231596352777E-6</v>
+      </c>
+      <c r="C197">
+        <v>2.4521231596352777E-6</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>2.4622013494372301</v>
+      </c>
+      <c r="B198">
+        <f t="shared" si="1"/>
+        <v>1.3494372299582835E-6</v>
+      </c>
+      <c r="C198">
+        <v>1.3494372299582835E-6</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>2.4622018830850698</v>
+      </c>
+      <c r="B199">
+        <f t="shared" si="1"/>
+        <v>1.8830850696538448E-6</v>
+      </c>
+      <c r="C199">
+        <v>1.8830850696538448E-6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>2.4622035394422701</v>
+      </c>
+      <c r="B200">
+        <f t="shared" si="1"/>
+        <v>3.539442269939741E-6</v>
+      </c>
+      <c r="C200">
+        <v>3.539442269939741E-6</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>2.4622057545930098</v>
+      </c>
+      <c r="B201">
+        <f t="shared" si="1"/>
+        <v>5.7545930096658537E-6</v>
+      </c>
+      <c r="C201">
+        <v>5.7545930096658537E-6</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>2.4622080475091899</v>
+      </c>
+      <c r="B202">
+        <f t="shared" si="1"/>
+        <v>8.0475091897014295E-6</v>
+      </c>
+      <c r="C202">
+        <v>8.0475091897014295E-6</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>2.4622099478728998</v>
+      </c>
+      <c r="B203">
+        <f t="shared" si="1"/>
+        <v>9.9478728996515997E-6</v>
+      </c>
+      <c r="C203">
+        <v>9.9478728996515997E-6</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>2.46221088152378</v>
+      </c>
+      <c r="B204">
+        <f t="shared" si="1"/>
+        <v>1.0881523779815439E-5</v>
+      </c>
+      <c r="C204">
+        <v>1.0881523779815439E-5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>2.4622102174907901</v>
+      </c>
+      <c r="B205">
+        <f t="shared" si="1"/>
+        <v>1.0217490789887762E-5</v>
+      </c>
+      <c r="C205">
+        <v>1.0217490789887762E-5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>2.4622077047824802</v>
+      </c>
+      <c r="B206">
+        <f t="shared" si="1"/>
+        <v>7.7047824800224873E-6</v>
+      </c>
+      <c r="C206">
+        <v>7.7047824800224873E-6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>2.4622042970731801</v>
+      </c>
+      <c r="B207">
+        <f t="shared" si="1"/>
+        <v>4.2970731799485407E-6</v>
+      </c>
+      <c r="C207">
+        <v>4.2970731799485407E-6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B208" s="24">
+        <f>AVERAGE($B$149:$B$207)</f>
+        <v>5.7688469806863088E-6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B209" s="24">
+        <f>MAX($B$149:$B$207)</f>
+        <v>1.0881523779815439E-5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B210" s="24">
+        <f>MIN($B$149:$B$207)</f>
+        <v>3.7993042978357039E-7</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B211" s="24">
+        <f>B209-B208</f>
+        <v>5.1126767991291297E-6</v>
+      </c>
+      <c r="C211" s="23">
+        <f>B211/A207</f>
+        <v>2.076463275288149E-6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B212" s="24">
+        <f>B211-B210</f>
+        <v>4.7327463693455594E-6</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B216" s="25"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>2458401.40555555</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>2458484.0277777701</v>
+      </c>
+      <c r="B218" s="26">
+        <f>A218-A217</f>
+        <v>82.622222220059484</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>2458566.74027777</v>
+      </c>
+      <c r="B219" s="26">
+        <f t="shared" ref="B219:B228" si="2">A219-A218</f>
+        <v>82.712499999906868</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>2458649.6722222199</v>
+      </c>
+      <c r="B220" s="26">
+        <f t="shared" si="2"/>
+        <v>82.931944449897856</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>2458732.86527777</v>
+      </c>
+      <c r="B221" s="26">
+        <f t="shared" si="2"/>
+        <v>83.193055550102144</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>2458816.26944444</v>
+      </c>
+      <c r="B222" s="26">
+        <f t="shared" si="2"/>
+        <v>83.404166670050472</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>2458899.7777777701</v>
+      </c>
+      <c r="B223" s="26">
+        <f t="shared" si="2"/>
+        <v>83.50833333004266</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>2458983.2888888801</v>
+      </c>
+      <c r="B224" s="26">
+        <f t="shared" si="2"/>
+        <v>83.511111109983176</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>2459066.7236111099</v>
+      </c>
+      <c r="B225" s="26">
+        <f t="shared" si="2"/>
+        <v>83.434722229838371</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>2459150.02222222</v>
+      </c>
+      <c r="B226" s="26">
+        <f t="shared" si="2"/>
+        <v>83.298611110076308</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>2459233.1486111102</v>
+      </c>
+      <c r="B227" s="26">
+        <f t="shared" si="2"/>
+        <v>83.126388890203089</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>2459316.0888888799</v>
+      </c>
+      <c r="B228" s="26">
+        <f t="shared" si="2"/>
+        <v>82.940277769695967</v>
       </c>
     </row>
   </sheetData>

</xml_diff>